<commit_message>
correction to laboratoire, 105% good job!
</commit_message>
<xml_diff>
--- a/LabsGrilleDeCorrection.xlsx
+++ b/LabsGrilleDeCorrection.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ccnbca-my.sharepoint.com/personal/dimitri_viel_ccnb_ca/Documents/Prog1343/Lab2 - Globex/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ccnbca-my.sharepoint.com/personal/dimitri_viel_ccnb_ca/Documents/Prog1343/Lab2 - Globex/Groupe1/Lab2-GlobeX-Groupe1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="53" documentId="8_{7AB2CD5E-D875-4634-96BE-3587703DCB10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2E104E26-3222-4CCF-8857-CB73E9047493}"/>
+  <xr:revisionPtr revIDLastSave="69" documentId="8_{7AB2CD5E-D875-4634-96BE-3587703DCB10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7FD88AB7-B176-462A-84EA-1A39805E5CC8}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{6E104A93-42AC-4B01-B277-A83AFE77E344}"/>
+    <workbookView xWindow="-54120" yWindow="10485" windowWidth="17595" windowHeight="19320" xr2:uid="{6E104A93-42AC-4B01-B277-A83AFE77E344}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>Exigences</t>
   </si>
@@ -93,6 +93,12 @@
   </si>
   <si>
     <t>Commentaires</t>
+  </si>
+  <si>
+    <t>**attention Radioactive Goods a le mauvais titre</t>
+  </si>
+  <si>
+    <t>** radioactive goods a le mauvais titre de page, les fields dans la form qui sont nécessaires devrais être noté (field required)</t>
   </si>
 </sst>
 </file>
@@ -450,7 +456,7 @@
   <dimension ref="A1:D34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -480,6 +486,9 @@
       <c r="B2">
         <v>1</v>
       </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
     </row>
     <row r="3" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
@@ -488,12 +497,18 @@
       <c r="B3">
         <v>8</v>
       </c>
+      <c r="C3">
+        <v>8</v>
+      </c>
     </row>
     <row r="4" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B4">
+        <v>2</v>
+      </c>
+      <c r="C4">
         <v>2</v>
       </c>
     </row>
@@ -504,6 +519,9 @@
       <c r="B5">
         <v>10</v>
       </c>
+      <c r="C5">
+        <v>10</v>
+      </c>
     </row>
     <row r="6" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
@@ -512,6 +530,12 @@
       <c r="B6">
         <v>10</v>
       </c>
+      <c r="C6">
+        <v>10</v>
+      </c>
+      <c r="D6" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="7" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
@@ -520,6 +544,9 @@
       <c r="B7">
         <v>10</v>
       </c>
+      <c r="C7">
+        <v>10</v>
+      </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
@@ -528,6 +555,9 @@
       <c r="B8">
         <v>10</v>
       </c>
+      <c r="C8">
+        <v>10</v>
+      </c>
     </row>
     <row r="9" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
@@ -536,6 +566,9 @@
       <c r="B9">
         <v>10</v>
       </c>
+      <c r="C9">
+        <v>10</v>
+      </c>
     </row>
     <row r="10" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
@@ -544,6 +577,9 @@
       <c r="B10">
         <v>5</v>
       </c>
+      <c r="C10">
+        <v>5</v>
+      </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
@@ -552,6 +588,9 @@
       <c r="B11">
         <v>10</v>
       </c>
+      <c r="C11">
+        <v>10</v>
+      </c>
     </row>
     <row r="12" spans="1:4" ht="75" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
@@ -560,6 +599,9 @@
       <c r="B12">
         <v>10</v>
       </c>
+      <c r="C12">
+        <v>10</v>
+      </c>
     </row>
     <row r="13" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
@@ -568,6 +610,9 @@
       <c r="B13">
         <v>10</v>
       </c>
+      <c r="C13">
+        <v>10</v>
+      </c>
     </row>
     <row r="14" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
@@ -576,6 +621,9 @@
       <c r="B14">
         <v>5</v>
       </c>
+      <c r="C14">
+        <v>5</v>
+      </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
@@ -587,7 +635,10 @@
       </c>
       <c r="C15">
         <f>SUM(C2:C14)</f>
-        <v>0</v>
+        <v>101</v>
+      </c>
+      <c r="D15" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -596,7 +647,7 @@
       </c>
       <c r="C16">
         <f>C15/B15*100</f>
-        <v>0</v>
+        <v>105.20833333333333</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">

</xml_diff>